<commit_message>
Change Sql Add Gui סיפורי משתמש 1 11 4 5 6 7 8 9 10 112 13 14 15 16 17 18 19 20 וכו'
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snirb\Dropbox\לימודים\סמי שמעון\שנה ב\סמסטר א\יסודות\פרויקט\Collind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA1F29-CBC8-4018-BAEA-22A4CB25CAF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC3C2C-2A17-4918-8AE8-6BD30AF304E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -179,6 +179,18 @@
   </si>
   <si>
     <t>Cube6</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>enable</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -523,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -745,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -772,6 +784,20 @@
       </c>
       <c r="H9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -789,15 +815,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -842,8 +868,11 @@
       <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -868,8 +897,11 @@
       <c r="H3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -894,8 +926,11 @@
       <c r="H4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -920,8 +955,11 @@
       <c r="H5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -946,8 +984,11 @@
       <c r="H6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -972,8 +1013,11 @@
       <c r="H7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -998,8 +1042,11 @@
       <c r="H8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1024,8 +1071,11 @@
       <c r="H9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1049,6 +1099,9 @@
       </c>
       <c r="H10" t="s">
         <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more gui Add images of screens exit סיפורי משתמש 1 11 4 5 6 7 8 9 10 112 13 14 15 16 17 18 19 20 וכו'
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1122,7 +1122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
@@ -1569,6 +1569,310 @@
         <v>9</v>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>8</v>
+      </c>
+      <c r="D26" t="n">
+        <v>9</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>9</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>9</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3</v>
+      </c>
+      <c r="D31" t="n">
+        <v>9</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" t="n">
+        <v>9</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>9</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>9</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>9</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>9</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>9</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>9</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>9</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>10.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>7</v>
+      </c>
+      <c r="D41" t="n">
+        <v>9</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>

</xml_diff>

<commit_message>
Added Print_User_List and feedback funcs to excelfunc add 1 unittest
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8964" windowWidth="18408" xWindow="3060" yWindow="3396"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cards" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Games" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cube" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cards" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Games" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Cube" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -21,14 +21,14 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <color theme="10"/>
       <sz val="11"/>
@@ -69,19 +69,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="היפר-קישור" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -347,26 +347,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="2.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="5.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.85546875" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.7109375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="2.59765625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="9.3984375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="8.69921875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="5.69921875"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="7.8984375"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="15.8984375"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" width="9.69921875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -797,7 +797,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>snirben</t>
+          <t>eladlp</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -807,7 +807,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>sdf</t>
+          <t>elad</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -833,13 +833,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -856,7 +856,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1212,18 +1212,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="2.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="6.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="9.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.42578125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="2.69921875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="6.8984375"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="9.296875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="9.3984375"/>
+    <col customWidth="1" max="5" min="5" width="16.796875"/>
+    <col customWidth="1" max="6" min="6" width="22.09765625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1247,6 +1249,16 @@
           <t>UserId</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>feedback</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1260,6 +1272,11 @@
       </c>
       <c r="D2" t="n">
         <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>it sucks</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -2026,7 +2043,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -2042,9 +2059,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="9.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="9.3984375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2120,6 +2137,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Gui of user storie 17,5 update wordinput
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Cards" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Games" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Cube" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cards" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Games" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cube" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -823,11 +823,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
add Gui of user storie 30 add func 30 to the main game
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8964" windowWidth="18408" xWindow="3060" yWindow="3396"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-15130" yWindow="1860" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Cards" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Games" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Cube" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cards" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Games" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cube" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -69,19 +69,19 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="היפר-קישור" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -358,15 +358,15 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="2.59765625"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="9.3984375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="8.69921875"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="5.69921875"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="7.8984375"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="15.8984375"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="9.69921875"/>
+    <col width="2.58203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="8.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="5.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="7.9140625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.9140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -833,13 +833,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -856,7 +856,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1212,20 +1212,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="2.69921875"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="6.8984375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="9.296875"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="9.3984375"/>
-    <col customWidth="1" max="5" min="5" width="16.796875"/>
-    <col customWidth="1" max="6" min="6" width="22.09765625"/>
+    <col width="2.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="6.9140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.83203125" customWidth="1" min="5" max="5"/>
+    <col width="22.08203125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1420,630 +1420,27 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>9</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>9</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>9</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" t="n">
-        <v>9</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>9</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>9</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="n">
-        <v>4</v>
-      </c>
-      <c r="D23" t="n">
-        <v>9</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>09.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>9</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="n">
-        <v>7</v>
-      </c>
-      <c r="C25" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" t="n">
-        <v>9</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="n">
-        <v>8</v>
-      </c>
-      <c r="D26" t="n">
-        <v>9</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>9</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>9</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="n">
-        <v>2</v>
-      </c>
-      <c r="D29" t="n">
-        <v>9</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>9</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>3</v>
-      </c>
-      <c r="D31" t="n">
-        <v>9</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" t="n">
-        <v>9</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>9</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>9</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>9</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>35</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>9</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>36</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>9</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>9</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>38</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>9</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>9</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="n">
-        <v>7</v>
-      </c>
-      <c r="D41" t="n">
-        <v>9</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>3</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>3</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>10.01.2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" t="n">
-        <v>4</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>11.01.2020</t>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>was ok</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2059,9 +1456,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="9.3984375"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2137,6 +1534,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add listOfUser function דרישה 6
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3060" yWindow="3396" windowWidth="18408" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -358,15 +358,15 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="2.59765625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.69921875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="5.69921875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="7.8984375" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.8984375" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.69921875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="2.58203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="8.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="5.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="7.9140625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.9140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -831,7 +831,46 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>tzlil</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>tzlil</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>levi</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>tzlil460@gmail</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>025</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
@@ -857,7 +896,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1213,20 +1252,20 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="2.69921875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="6.8984375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="9.296875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="16.796875" customWidth="1" min="5" max="5"/>
-    <col width="22.09765625" customWidth="1" min="6" max="6"/>
+    <col width="2.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="6.9140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.83203125" customWidth="1" min="5" max="5"/>
+    <col width="22.08203125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2040,6 +2079,187 @@
       <c r="E44" t="inlineStr">
         <is>
           <t>11.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>9</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>9</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>9</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>9</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>5</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" t="n">
+        <v>9</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>7</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="n">
+        <v>9</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" t="n">
+        <v>5</v>
+      </c>
+      <c r="D52" t="n">
+        <v>9</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>i like this game</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" t="n">
+        <v>6</v>
+      </c>
+      <c r="D53" t="n">
+        <v>3</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>12.01.2020</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>אין</t>
         </is>
       </c>
     </row>
@@ -2060,9 +2280,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add Report TO SQL userstore 5, 10, 13
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snirb\Dropbox\לימודים\סמי שמעון\שנה ב\סמסטר א\יסודות\פרויקט\Collind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934B2E40-C5A4-4DE3-81E9-44E82BF634B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D98F2B2-B1CF-4E20-9D80-C9EB4A3C3BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -292,6 +292,18 @@
               You can use visual aids, apps, and other technology to help you live with color blindness.  \
               For example, you can use an app to take a photo with your phone or tablet and then tap on part of the  \
               photo to find out the color of that area. </t>
+  </si>
+  <si>
+    <t>Diagnose</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>deficient</t>
+  </si>
+  <si>
+    <t>badly worsened</t>
   </si>
 </sst>
 </file>
@@ -2303,47 +2315,60 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7640A13-9EEC-4754-81BB-13186A552440}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="80.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="52" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="52" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="84" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="84" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user storie 2 upgrade to unit testing
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1274,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -2282,6 +2282,177 @@
       <c r="F53" t="inlineStr">
         <is>
           <t>אין</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>3</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>3</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Problem with screen of the reportS FIX unittest
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -1274,7 +1274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -2451,6 +2451,63 @@
         <v>3</v>
       </c>
       <c r="E62" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>3</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>14.01.2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>3</v>
+      </c>
+      <c r="E65" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>

</xml_diff>

<commit_message>
Change names of func to match dfd add Unittests
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -37,24 +37,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <color rgb="FFA9B7C6"/>
-      <sz val="9.800000000000001"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <family val="3"/>
-      <color rgb="FF6A8759"/>
-      <sz val="9.800000000000001"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="9"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.3499862666707358"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -85,23 +85,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -376,518 +382,521 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="2.59765625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="2.8984375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="9.3984375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.69921875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="5.69921875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="7.8984375" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.8984375" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.69921875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="8.796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="7.19921875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.09765625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.69921875" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.8984375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="5.69921875" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>UserName</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>lastname</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>phone</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>team7@gmail.com</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="1" t="n">
         <v>543149811</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>tzlille</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>levi</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>tzlil@com</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="1" t="inlineStr">
         <is>
           <t>053446</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>tester</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>tester</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>team7@gmail.com</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="1" t="n">
         <v>3556</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>tester</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>jennia</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>team7@gmail.com</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="1" t="n">
         <v>1111</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>elad</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>team7</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>team7@gmail.com</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="1" t="n">
         <v>56756</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>neta</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>levi</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="1" t="inlineStr">
         <is>
           <t>tzlil@com</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="1" t="inlineStr">
         <is>
           <t>053446</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>tzlille</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="1" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="1" t="inlineStr">
         <is>
           <t>levi</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="1" t="inlineStr">
         <is>
           <t>tzlil@com</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="1" t="inlineStr">
         <is>
           <t>053446</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="1" t="inlineStr">
         <is>
           <t>neta</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="1" t="inlineStr">
         <is>
           <t>abcd</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="1" t="inlineStr">
         <is>
           <t>levi</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="1" t="inlineStr">
         <is>
           <t>tzlil@com</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="1" t="inlineStr">
         <is>
           <t>053446</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="1" t="inlineStr">
         <is>
           <t>testtes</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="1" t="inlineStr">
         <is>
           <t>test</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="1" t="inlineStr">
         <is>
           <t>43</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="1" t="inlineStr">
         <is>
           <t>sdfsdf</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="1" t="inlineStr">
         <is>
           <t>asdfsad</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="1" t="inlineStr">
         <is>
           <t>asd</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="1" t="inlineStr">
         <is>
           <t>asd</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="1" t="inlineStr">
         <is>
           <t>231</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="1" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="1" t="inlineStr">
         <is>
           <t>eladlp</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="1" t="inlineStr">
         <is>
           <t>24234</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="1" t="inlineStr">
         <is>
           <t>elad</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="1" t="inlineStr">
         <is>
           <t>sdf</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="1" t="inlineStr">
         <is>
           <t>sdf</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="1" t="inlineStr">
         <is>
           <t>sdf</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" s="1" t="inlineStr">
         <is>
           <t>sdf</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="1" t="inlineStr">
         <is>
           <t>tzlil</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="1" t="inlineStr">
         <is>
           <t>levi</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="1" t="inlineStr">
         <is>
           <t>tzlil460@gmail</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="1" t="inlineStr">
         <is>
           <t>025</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="1" t="inlineStr">
         <is>
           <t>user</t>
         </is>
@@ -915,54 +924,60 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>כוכב</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>עיגול</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>ריבוע</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>לב</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>ירח</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>משולש</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="n"/>
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>A</t>
@@ -993,14 +1008,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -1021,19 +1033,19 @@
       <c r="G3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>CARD1</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>yes</t>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -1054,19 +1066,19 @@
       <c r="G4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>CARD2</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -1087,19 +1099,19 @@
       <c r="G5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>CARD3</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -1120,19 +1132,19 @@
       <c r="G6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>CARD4</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="1" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
@@ -1153,19 +1165,19 @@
       <c r="G7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="1" t="inlineStr">
         <is>
           <t>CARD5</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="1" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
@@ -1186,19 +1198,19 @@
       <c r="G8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="1" t="inlineStr">
         <is>
           <t>CARD6</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="1" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
@@ -1219,19 +1231,19 @@
       <c r="G9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="1" t="inlineStr">
         <is>
           <t>CARD7</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="1" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
@@ -1252,12 +1264,12 @@
       <c r="G10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="1" t="inlineStr">
         <is>
           <t>CARD8</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="1" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1274,10 +1286,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
@@ -1291,1225 +1303,1457 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">correct </t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>not correct</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>UserId</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>feedback</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>it sucks</t>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Ok</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>09.01.2020</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F10" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9</v>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F11" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>9</v>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>9</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>9</v>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F15" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>9</v>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="B16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>9</v>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F17" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="B18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="D18" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="D18" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" t="n">
-        <v>9</v>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F19" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D20" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="D20" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>9</v>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="B21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F21" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>9</v>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="B22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" t="n">
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D23" t="n">
-        <v>9</v>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="D23" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
         <is>
           <t>09.01.2020</t>
         </is>
       </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>9</v>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="B24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C25" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" t="n">
-        <v>9</v>
-      </c>
-      <c r="E25" t="inlineStr">
+      <c r="C25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="n">
+      <c r="B26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D26" t="n">
-        <v>9</v>
-      </c>
-      <c r="E26" t="inlineStr">
+      <c r="D26" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>9</v>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="B27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F27" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>9</v>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="B28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" t="n">
+      <c r="B29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D29" t="n">
-        <v>9</v>
-      </c>
-      <c r="E29" t="inlineStr">
+      <c r="D29" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>9</v>
-      </c>
-      <c r="E30" t="inlineStr">
+      <c r="B30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>אין</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>3</v>
-      </c>
-      <c r="D31" t="n">
-        <v>9</v>
-      </c>
-      <c r="E31" t="inlineStr">
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F31" s="1" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C32" t="n">
+      <c r="B32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D32" t="n">
-        <v>9</v>
-      </c>
-      <c r="E32" t="inlineStr">
+      <c r="D32" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F32" s="1" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>9</v>
-      </c>
-      <c r="E33" t="inlineStr">
+      <c r="B33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F33" s="1" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" t="n">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>9</v>
-      </c>
-      <c r="E34" t="inlineStr">
+      <c r="B34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F34" s="1" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" t="n">
+      <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>9</v>
-      </c>
-      <c r="E35" t="inlineStr">
+      <c r="B35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F35" s="1" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>9</v>
-      </c>
-      <c r="E36" t="inlineStr">
+      <c r="B36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>9</v>
-      </c>
-      <c r="E37" t="inlineStr">
+      <c r="B37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F37" s="1" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>9</v>
-      </c>
-      <c r="E38" t="inlineStr">
+      <c r="B38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F38" s="1" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>9</v>
-      </c>
-      <c r="E39" t="inlineStr">
+      <c r="B39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F39" s="1" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>9</v>
-      </c>
-      <c r="E40" t="inlineStr">
+      <c r="B40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F40" s="1" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="n">
+      <c r="B41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D41" t="n">
-        <v>9</v>
-      </c>
-      <c r="E41" t="inlineStr">
+      <c r="D41" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F41" s="1" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>3</v>
-      </c>
-      <c r="E42" t="inlineStr">
+      <c r="B42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F42" s="1" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>3</v>
-      </c>
-      <c r="E43" t="inlineStr">
+      <c r="B43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
         <is>
           <t>10.01.2020</t>
         </is>
       </c>
+      <c r="F43" s="1" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" t="inlineStr">
+      <c r="C44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
         <is>
           <t>11.01.2020</t>
         </is>
       </c>
+      <c r="F44" s="1" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" t="n">
+      <c r="B45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D45" t="n">
-        <v>3</v>
-      </c>
-      <c r="E45" t="inlineStr">
+      <c r="D45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F45" s="1" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" t="n">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>9</v>
-      </c>
-      <c r="E46" t="inlineStr">
+      <c r="B46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F46" s="1" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>9</v>
-      </c>
-      <c r="E47" t="inlineStr">
+      <c r="B47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F47" s="1" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" t="n">
+      <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="n">
-        <v>9</v>
-      </c>
-      <c r="E48" t="inlineStr">
+      <c r="B48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F48" s="1" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>9</v>
-      </c>
-      <c r="E49" t="inlineStr">
+      <c r="B49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F49" s="1" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" t="n">
+      <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C50" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" t="n">
-        <v>9</v>
-      </c>
-      <c r="E50" t="inlineStr">
+      <c r="C50" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F50" s="1" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" t="n">
+      <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C51" t="n">
-        <v>1</v>
-      </c>
-      <c r="D51" t="n">
-        <v>9</v>
-      </c>
-      <c r="E51" t="inlineStr">
+      <c r="C51" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
+      <c r="F51" s="1" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" t="n">
+      <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B52" t="n">
-        <v>3</v>
-      </c>
-      <c r="C52" t="n">
+      <c r="B52" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D52" t="n">
-        <v>9</v>
-      </c>
-      <c r="E52" t="inlineStr">
+      <c r="D52" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E52" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" s="1" t="inlineStr">
         <is>
           <t>i like this game</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
+      <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B53" t="n">
-        <v>3</v>
-      </c>
-      <c r="C53" t="n">
+      <c r="B53" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D53" t="n">
-        <v>3</v>
-      </c>
-      <c r="E53" t="inlineStr">
+      <c r="D53" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
         <is>
           <t>12.01.2020</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" s="1" t="inlineStr">
         <is>
           <t>אין</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
+      <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>3</v>
-      </c>
-      <c r="E54" t="inlineStr">
+      <c r="B54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F54" s="1" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" t="n">
+      <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B55" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
-        <v>3</v>
-      </c>
-      <c r="E55" t="inlineStr">
+      <c r="B55" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F55" s="1" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" t="n">
+      <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B56" t="n">
-        <v>0</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" t="n">
-        <v>3</v>
-      </c>
-      <c r="E56" t="inlineStr">
+      <c r="B56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F56" s="1" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" t="n">
+      <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B57" t="n">
-        <v>0</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
-        <v>3</v>
-      </c>
-      <c r="E57" t="inlineStr">
+      <c r="B57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F57" s="1" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" t="n">
+      <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B58" t="n">
-        <v>0</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" t="n">
-        <v>3</v>
-      </c>
-      <c r="E58" t="inlineStr">
+      <c r="B58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F58" s="1" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" t="n">
+      <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B59" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="n">
-        <v>3</v>
-      </c>
-      <c r="E59" t="inlineStr">
+      <c r="B59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F59" s="1" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" t="n">
+      <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B60" t="n">
-        <v>0</v>
-      </c>
-      <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" t="inlineStr">
+      <c r="B60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F60" s="1" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" t="n">
+      <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B61" t="n">
-        <v>0</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
-        <v>3</v>
-      </c>
-      <c r="E61" t="inlineStr">
+      <c r="B61" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F61" s="1" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" t="n">
+      <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B62" t="n">
-        <v>0</v>
-      </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="n">
-        <v>3</v>
-      </c>
-      <c r="E62" t="inlineStr">
+      <c r="B62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F62" s="1" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" t="n">
+      <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B63" t="n">
-        <v>0</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="n">
-        <v>3</v>
-      </c>
-      <c r="E63" t="inlineStr">
+      <c r="B63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F63" s="1" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" t="n">
+      <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B64" t="n">
-        <v>0</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" t="n">
-        <v>3</v>
-      </c>
-      <c r="E64" t="inlineStr">
+      <c r="B64" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
         </is>
       </c>
+      <c r="F64" s="1" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" t="n">
+      <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B65" t="n">
-        <v>0</v>
-      </c>
-      <c r="C65" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" t="n">
-        <v>3</v>
-      </c>
-      <c r="E65" t="inlineStr">
+      <c r="B65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E65" s="1" t="inlineStr">
         <is>
           <t>14.01.2020</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>17.01.2020</t>
         </is>
       </c>
     </row>
@@ -2527,21 +2771,22 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.3984375" customWidth="1" min="1" max="1"/>
+    <col width="15.69921875" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Pic</t>
         </is>
@@ -2573,7 +2818,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cube3</t>
+          <t>Cube3.png</t>
         </is>
       </c>
     </row>
@@ -2583,7 +2828,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cube4</t>
+          <t>Cube4.png</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2838,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cube5</t>
+          <t>Cube5.png</t>
         </is>
       </c>
     </row>
@@ -2603,7 +2848,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cube6</t>
+          <t>Cube6.png</t>
         </is>
       </c>
     </row>
@@ -2618,10 +2863,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
@@ -2631,17 +2876,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Msg</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Diagnose</t>
         </is>
@@ -2651,9 +2896,9 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>check</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Your color vision regarded as normal.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2666,11 +2911,10 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Your color vision regarded as deficient.  \
-              Special contact lenses and glasses may help people who are color blind tell the difference between  \
-              colors. </t>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your color vision regarded as deficient. 
+Special contact lenses and glasses may help people who are color blind tell the difference between colors. </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2683,9 +2927,10 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>Your vision is shit</t>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your color vision regarded as badly worsen.  You can use visual aids, apps, and other technology to help you live with color blindness.  
+For example, you can use an app to take a photo with your phone or tablet and then tap on part of the photo to find out the color of that area. </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2693,6 +2938,15 @@
           <t>badly worsened</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Last Changed to UnitTesting. and resetUser func.
</commit_message>
<xml_diff>
--- a/gameSQL.xlsx
+++ b/gameSQL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" state="visible" r:id="rId1"/>
@@ -382,20 +382,20 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="2.8984375" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="8.796875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="7.19921875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="8.09765625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.69921875" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="9.8984375" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="5.69921875" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="2.9140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="8.83203125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="7.1640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.08203125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.6640625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="9.9140625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="5.6640625" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -927,7 +927,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="inlineStr">
@@ -1288,18 +1288,18 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="2.69921875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="6.8984375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="9.296875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9.3984375" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="16.796875" customWidth="1" min="5" max="5"/>
-    <col width="22.09765625" customWidth="1" min="6" max="6"/>
+    <col width="2.6640625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="6.9140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="9.4140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.83203125" customWidth="1" min="5" max="5"/>
+    <col width="22.08203125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1849,7 +1849,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
@@ -2035,7 +2035,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>3</v>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="E42" s="1" t="inlineStr">
         <is>
-          <t>10.01.2020</t>
+          <t>17.01.2020</t>
         </is>
       </c>
       <c r="F42" s="1" t="n"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="E43" s="1" t="inlineStr">
         <is>
-          <t>10.01.2020</t>
+          <t>17.01.2020</t>
         </is>
       </c>
       <c r="F43" s="1" t="n"/>
@@ -2315,17 +2315,17 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="inlineStr">
         <is>
-          <t>12.01.2020</t>
+          <t>11.01.2020</t>
         </is>
       </c>
       <c r="F45" s="1" t="n"/>
@@ -2479,24 +2479,20 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E53" s="1" t="inlineStr">
         <is>
-          <t>12.01.2020</t>
-        </is>
-      </c>
-      <c r="F53" s="1" t="inlineStr">
-        <is>
-          <t>אין</t>
-        </is>
-      </c>
+          <t>17.01.2020</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2513,7 +2509,7 @@
       </c>
       <c r="E54" s="1" t="inlineStr">
         <is>
-          <t>14.01.2020</t>
+          <t>17.01.2020</t>
         </is>
       </c>
       <c r="F54" s="1" t="n"/>
@@ -2533,209 +2529,89 @@
       </c>
       <c r="E55" s="1" t="inlineStr">
         <is>
-          <t>14.01.2020</t>
+          <t>17.01.2020</t>
         </is>
       </c>
       <c r="F55" s="1" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A56" s="1" t="n"/>
+      <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
+      <c r="E56" s="1" t="n"/>
       <c r="F56" s="1" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E57" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A57" s="1" t="n"/>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="n"/>
+      <c r="D57" s="1" t="n"/>
+      <c r="E57" s="1" t="n"/>
       <c r="F57" s="1" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B58" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E58" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A58" s="1" t="n"/>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="n"/>
+      <c r="D58" s="1" t="n"/>
+      <c r="E58" s="1" t="n"/>
       <c r="F58" s="1" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B59" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E59" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A59" s="1" t="n"/>
+      <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
+      <c r="E59" s="1" t="n"/>
       <c r="F59" s="1" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E60" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A60" s="1" t="n"/>
+      <c r="B60" s="1" t="n"/>
+      <c r="C60" s="1" t="n"/>
+      <c r="D60" s="1" t="n"/>
+      <c r="E60" s="1" t="n"/>
       <c r="F60" s="1" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E61" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A61" s="1" t="n"/>
+      <c r="B61" s="1" t="n"/>
+      <c r="C61" s="1" t="n"/>
+      <c r="D61" s="1" t="n"/>
+      <c r="E61" s="1" t="n"/>
       <c r="F61" s="1" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E62" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A62" s="1" t="n"/>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
+      <c r="E62" s="1" t="n"/>
       <c r="F62" s="1" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E63" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A63" s="1" t="n"/>
+      <c r="B63" s="1" t="n"/>
+      <c r="C63" s="1" t="n"/>
+      <c r="D63" s="1" t="n"/>
+      <c r="E63" s="1" t="n"/>
       <c r="F63" s="1" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E64" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="n"/>
+      <c r="D64" s="1" t="n"/>
+      <c r="E64" s="1" t="n"/>
       <c r="F64" s="1" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E65" s="1" t="inlineStr">
-        <is>
-          <t>14.01.2020</t>
-        </is>
-      </c>
+      <c r="A65" s="1" t="n"/>
+      <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="n"/>
+      <c r="D65" s="1" t="n"/>
+      <c r="E65" s="1" t="n"/>
       <c r="F65" s="1" t="n"/>
     </row>
     <row r="66">
@@ -2774,10 +2650,10 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="11.3984375" customWidth="1" min="1" max="1"/>
-    <col width="15.69921875" customWidth="1" min="2" max="2"/>
+    <col width="11.4140625" customWidth="1" min="1" max="1"/>
+    <col width="15.6640625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2869,10 +2745,10 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col width="80.09765625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13.296875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="80.08203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2923,7 +2799,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="82.8" customHeight="1">
+    <row r="4" ht="82.75" customHeight="1">
       <c r="A4" t="n">
         <v>3</v>
       </c>

</xml_diff>